<commit_message>
Did handsOn for intern
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFramework/resources/testData.xlsx
+++ b/SeleniumAutomationFramework/resources/testData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HI\My_Items\Job\Softwares\eclipse-workspace3\SeleniumAutomationFramework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEA48C4-B182-45C0-9686-62AAB4FC5FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D4D6D0-F8F6-40D1-B205-41416100928F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Keyword</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -43,12 +37,25 @@
   </si>
   <si>
     <t>search</t>
+  </si>
+  <si>
+    <t>yousuf</t>
+  </si>
+  <si>
+    <t>riyak</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>FAILED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -360,46 +367,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0">
+        <v>793206</v>
+      </c>
+      <c r="C2" t="b" s="0">
         <v>1</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
+      <c r="A3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0">
+        <v>110223</v>
+      </c>
+      <c r="C3" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>